<commit_message>
updated results excel sheet
</commit_message>
<xml_diff>
--- a/AnalysisOfResults.xlsx
+++ b/AnalysisOfResults.xlsx
@@ -5,27 +5,33 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Burruss\Documents\Modeling and Simulation\Final Project\Netlogo-Horse-Race-Simulator-Gambling-Predictor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Documents\Netlogo-Horse-Race-Simulator-Gambling-Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1629E51-DE48-4150-BD42-46CAC57BC15D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C088972F-B74B-4E0A-A854-DDB07DF8E65F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2760" windowWidth="29040" windowHeight="15840" xr2:uid="{93AD6383-F7CA-4432-931A-A13690181AA1}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{93AD6383-F7CA-4432-931A-A13690181AA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="37">
   <si>
     <t>Dataset</t>
   </si>
@@ -91,17 +97,70 @@
   </si>
   <si>
     <t>Dancing Starlet</t>
+  </si>
+  <si>
+    <t>Bronzed</t>
+  </si>
+  <si>
+    <t>Math Wizard</t>
+  </si>
+  <si>
+    <t>Gran Paraiso</t>
+  </si>
+  <si>
+    <t>Joe DiBaggio</t>
+  </si>
+  <si>
+    <t>Tiger Blood</t>
+  </si>
+  <si>
+    <t>Giant's Voice</t>
+  </si>
+  <si>
+    <t>Dance Proudly</t>
+  </si>
+  <si>
+    <t>Captain Gaughen</t>
+  </si>
+  <si>
+    <t>Hardened</t>
+  </si>
+  <si>
+    <t>Polar Jet</t>
+  </si>
+  <si>
+    <t>I Idolize You</t>
+  </si>
+  <si>
+    <t>Coop Tries Harder</t>
+  </si>
+  <si>
+    <t>Souper Stonehenge</t>
+  </si>
+  <si>
+    <t>Salambo</t>
+  </si>
+  <si>
+    <t>Running for Riz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,27 +408,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -378,27 +426,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -410,9 +437,6 @@
     <xf numFmtId="6" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -421,12 +445,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -460,22 +478,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -486,18 +489,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -516,8 +507,81 @@
     <xf numFmtId="6" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -832,497 +896,618 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19A948A-A305-4899-B78B-C7689B191CE0}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83984375" customWidth="1"/>
+    <col min="3" max="3" width="9.83984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.41796875" customWidth="1"/>
+    <col min="9" max="9" width="9.26171875" customWidth="1"/>
+    <col min="11" max="11" width="9.578125" customWidth="1"/>
+    <col min="12" max="12" width="12.578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.68359375" customWidth="1"/>
+    <col min="15" max="15" width="12.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="1:16" ht="29.1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="24"/>
+      <c r="B1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="57" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="42"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="40"/>
+      <c r="M2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="43"/>
+      <c r="N2" s="41"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="42">
+    <row r="3" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="44" t="s">
-        <v>13</v>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="58" t="s">
+        <v>12</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="42">
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="44"/>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="58" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="42">
+    <row r="5" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="44"/>
+      <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="58" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="42">
+    <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="44" t="s">
+      <c r="K6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="58" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45">
+    <row r="7" spans="1:16" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="26">
         <v>5</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="51" t="s">
+      <c r="J7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="N7" s="52" t="s">
+      <c r="K7" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="59" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:16" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+    <row r="8" spans="1:16" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="53"/>
+    </row>
+    <row r="10" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="53"/>
+    </row>
+    <row r="11" spans="1:16" ht="29.1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="24" t="s">
+      <c r="K11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="L11" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="26"/>
+      <c r="M11" s="38"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21" t="s">
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21" t="s">
+      <c r="G12" s="36"/>
+      <c r="H12" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21" t="s">
+      <c r="I12" s="36"/>
+      <c r="J12" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="21"/>
-      <c r="L12" s="18" t="s">
+      <c r="K12" s="36"/>
+      <c r="L12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="13">
         <v>1</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="3">
-        <f t="shared" ref="L13:L16" si="0">SUM(B13,D13,F13,H13,J13)</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="29">
+      <c r="B13" s="43">
+        <v>-2</v>
+      </c>
+      <c r="C13" s="44">
+        <v>-2</v>
+      </c>
+      <c r="D13" s="43">
+        <v>-2</v>
+      </c>
+      <c r="E13" s="45">
+        <v>-2</v>
+      </c>
+      <c r="F13" s="46">
+        <v>4.8</v>
+      </c>
+      <c r="G13" s="45">
+        <v>-2</v>
+      </c>
+      <c r="H13" s="43">
+        <v>-4</v>
+      </c>
+      <c r="I13" s="45">
+        <v>-4</v>
+      </c>
+      <c r="J13" s="46">
+        <v>-12</v>
+      </c>
+      <c r="K13" s="45">
+        <v>-12</v>
+      </c>
+      <c r="L13" s="47">
+        <f t="shared" ref="L13:L15" si="0">SUM(B13,D13,F13,H13,J13)</f>
+        <v>-15.2</v>
+      </c>
+      <c r="M13" s="48">
         <f>SUM(C13,E13,G13,I13,K13)</f>
-        <v>0</v>
+        <v>-22</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="13">
         <v>2</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="3">
+      <c r="B14" s="49">
+        <v>-2</v>
+      </c>
+      <c r="C14" s="50">
+        <v>5</v>
+      </c>
+      <c r="D14" s="49">
+        <v>2.6</v>
+      </c>
+      <c r="E14" s="51">
+        <v>-2</v>
+      </c>
+      <c r="F14" s="52">
+        <v>2.6</v>
+      </c>
+      <c r="G14" s="51">
+        <v>2.1</v>
+      </c>
+      <c r="H14" s="52">
+        <v>8.6</v>
+      </c>
+      <c r="I14" s="51">
+        <v>-4</v>
+      </c>
+      <c r="J14" s="52">
+        <v>19.2</v>
+      </c>
+      <c r="K14" s="51">
+        <v>-12</v>
+      </c>
+      <c r="L14" s="47">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="29">
+        <v>31</v>
+      </c>
+      <c r="M14" s="48">
         <f t="shared" ref="M14:M16" si="1">SUM(C14,E14,G14,I14,K14)</f>
-        <v>0</v>
+        <v>-10.9</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="13">
         <v>3</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="3">
+      <c r="B15" s="49">
+        <v>-2</v>
+      </c>
+      <c r="C15" s="50">
+        <v>-2</v>
+      </c>
+      <c r="D15" s="49">
+        <v>5</v>
+      </c>
+      <c r="E15" s="51">
+        <v>-2</v>
+      </c>
+      <c r="F15" s="52">
+        <v>-2</v>
+      </c>
+      <c r="G15" s="51">
+        <v>3.6</v>
+      </c>
+      <c r="H15" s="52">
+        <v>-4</v>
+      </c>
+      <c r="I15" s="51">
+        <v>-4</v>
+      </c>
+      <c r="J15" s="52">
+        <v>-12</v>
+      </c>
+      <c r="K15" s="51">
+        <v>-12</v>
+      </c>
+      <c r="L15" s="47">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="29">
+        <v>-15</v>
+      </c>
+      <c r="M15" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-16.399999999999999</v>
       </c>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="13">
         <v>4</v>
       </c>
-      <c r="B16" s="17">
-        <v>-2</v>
-      </c>
-      <c r="C16" s="20">
-        <v>-2</v>
-      </c>
-      <c r="D16" s="53">
+      <c r="B16" s="6">
+        <v>-2</v>
+      </c>
+      <c r="C16" s="9">
+        <v>-2</v>
+      </c>
+      <c r="D16" s="30">
         <v>3.6</v>
       </c>
-      <c r="E16" s="55">
-        <v>-2</v>
-      </c>
-      <c r="F16" s="54">
-        <v>-2</v>
-      </c>
-      <c r="G16" s="56">
+      <c r="E16" s="32">
+        <v>-2</v>
+      </c>
+      <c r="F16" s="31">
+        <v>-2</v>
+      </c>
+      <c r="G16" s="33">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H16" s="54">
+      <c r="H16" s="31">
         <v>-4</v>
       </c>
-      <c r="I16" s="54">
+      <c r="I16" s="31">
         <v>-4</v>
       </c>
-      <c r="J16" s="54">
+      <c r="J16" s="31">
         <v>-12</v>
       </c>
-      <c r="K16" s="54">
+      <c r="K16" s="31">
         <v>-12</v>
       </c>
-      <c r="L16" s="19">
+      <c r="L16" s="8">
         <f>SUM(B16,D16,F16,H16,J16)</f>
         <v>-16.399999999999999</v>
       </c>
-      <c r="M16" s="29">
+      <c r="M16" s="15">
         <f t="shared" si="1"/>
         <v>-17.8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30">
+    <row r="17" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="16">
         <v>5</v>
       </c>
-      <c r="B17" s="57">
-        <v>-2</v>
-      </c>
-      <c r="C17" s="58">
-        <v>-2</v>
-      </c>
-      <c r="D17" s="31">
-        <v>-2</v>
-      </c>
-      <c r="E17" s="32">
+      <c r="B17" s="34">
+        <v>-2</v>
+      </c>
+      <c r="C17" s="35">
+        <v>-2</v>
+      </c>
+      <c r="D17" s="17">
+        <v>-2</v>
+      </c>
+      <c r="E17" s="18">
         <v>10.4</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="20">
         <v>3</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="17">
         <v>-4</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="20">
         <v>-4</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="21">
         <v>-12</v>
       </c>
-      <c r="K17" s="34">
+      <c r="K17" s="20">
         <v>964</v>
       </c>
-      <c r="L17" s="36">
+      <c r="L17" s="22">
         <f>SUM(B17,D17,F17,H17,J17)</f>
         <v>-17.8</v>
       </c>
-      <c r="M17" s="37">
+      <c r="M17" s="23">
         <f>SUM(C17,E17,G17,I17,K17)</f>
         <v>971.4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
@@ -1330,10 +1515,6 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="J12:K12"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>